<commit_message>
added laborproductivity for 2015
</commit_message>
<xml_diff>
--- a/Documentation/DataV3.xlsx
+++ b/Documentation/DataV3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Region</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>LaborProductivity2012</t>
+  </si>
+  <si>
+    <t>LaborProductivity2015</t>
   </si>
 </sst>
 </file>
@@ -592,11 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I6" sqref="I6"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,9 +620,10 @@
     <col min="16" max="16" width="26.5703125" customWidth="1"/>
     <col min="17" max="17" width="26.42578125" customWidth="1"/>
     <col min="18" max="18" width="27.5703125" customWidth="1"/>
+    <col min="19" max="19" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -674,8 +678,11 @@
       <c r="R1" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="S1" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -736,8 +743,11 @@
       <c r="R2" s="11">
         <v>501123</v>
       </c>
+      <c r="S2" s="11">
+        <v>583368</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -798,8 +808,11 @@
       <c r="R3" s="11">
         <v>103184</v>
       </c>
+      <c r="S3" s="4">
+        <v>117327</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -860,8 +873,11 @@
       <c r="R4" s="11">
         <v>162642</v>
       </c>
+      <c r="S4" s="4">
+        <v>175870</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -922,8 +938,11 @@
       <c r="R5" s="11">
         <v>78027</v>
       </c>
+      <c r="S5" s="4">
+        <v>88532</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -984,8 +1003,11 @@
       <c r="R6" s="11">
         <v>151196</v>
       </c>
+      <c r="S6" s="4">
+        <v>170684</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
@@ -1046,8 +1068,11 @@
       <c r="R7" s="11">
         <v>230968</v>
       </c>
+      <c r="S7" s="4">
+        <v>256386</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>49</v>
       </c>
@@ -1108,8 +1133,11 @@
       <c r="R8" s="11">
         <v>8618</v>
       </c>
+      <c r="S8" s="4">
+        <v>94144</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -1170,8 +1198,11 @@
       <c r="R9" s="11">
         <v>55798</v>
       </c>
+      <c r="S9" s="4">
+        <v>65196</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -1232,8 +1263,11 @@
       <c r="R10" s="11">
         <v>85834</v>
       </c>
+      <c r="S10" s="4">
+        <v>95211</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
@@ -1294,8 +1328,11 @@
       <c r="R11" s="11">
         <v>135996</v>
       </c>
+      <c r="S11" s="4">
+        <v>150228</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -1356,8 +1393,11 @@
       <c r="R12" s="11">
         <v>80982</v>
       </c>
+      <c r="S12" s="4">
+        <v>150555</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>21</v>
       </c>
@@ -1418,8 +1458,11 @@
       <c r="R13" s="11">
         <v>94907</v>
       </c>
+      <c r="S13" s="4">
+        <v>113384</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1480,8 +1523,11 @@
       <c r="R14" s="11">
         <v>121499</v>
       </c>
+      <c r="S14" s="4">
+        <v>142402</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>25</v>
       </c>
@@ -1542,8 +1588,11 @@
       <c r="R15" s="11">
         <v>128692</v>
       </c>
+      <c r="S15" s="4">
+        <v>157780</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -1604,8 +1653,11 @@
       <c r="R16" s="11">
         <v>101590</v>
       </c>
+      <c r="S16" s="4">
+        <v>115772</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
@@ -1666,8 +1718,11 @@
       <c r="R17" s="11">
         <v>75024</v>
       </c>
+      <c r="S17" s="4">
+        <v>88178</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
@@ -1727,6 +1782,9 @@
       </c>
       <c r="R18" s="11">
         <v>38647</v>
+      </c>
+      <c r="S18" s="4">
+        <v>40008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor change in DataV3
</commit_message>
<xml_diff>
--- a/Documentation/DataV3.xlsx
+++ b/Documentation/DataV3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\IBMDESC-Poverty\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Desktop\IBMDESC-Poverty\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -254,7 +254,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,7 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -598,8 +597,8 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S1" sqref="S1"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +739,10 @@
       <c r="Q2" s="4">
         <v>25007</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="4">
         <v>501123</v>
       </c>
-      <c r="S2" s="11">
+      <c r="S2" s="4">
         <v>583368</v>
       </c>
     </row>
@@ -805,7 +804,7 @@
       <c r="Q3" s="4">
         <v>20448</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="4">
         <v>103184</v>
       </c>
       <c r="S3" s="4">
@@ -870,7 +869,7 @@
       <c r="Q4" s="4">
         <v>21770</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="4">
         <v>162642</v>
       </c>
       <c r="S4" s="4">
@@ -935,7 +934,7 @@
       <c r="Q5" s="4">
         <v>21860</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="4">
         <v>78027</v>
       </c>
       <c r="S5" s="4">
@@ -1000,7 +999,7 @@
       <c r="Q6" s="4">
         <v>23200</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6" s="4">
         <v>151196</v>
       </c>
       <c r="S6" s="4">
@@ -1065,7 +1064,7 @@
       <c r="Q7" s="4">
         <v>22121</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="4">
         <v>230968</v>
       </c>
       <c r="S7" s="4">
@@ -1130,7 +1129,7 @@
       <c r="Q8" s="4">
         <v>20224</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="4">
         <v>8618</v>
       </c>
       <c r="S8" s="4">
@@ -1195,7 +1194,7 @@
       <c r="Q9" s="4">
         <v>21476</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="4">
         <v>55798</v>
       </c>
       <c r="S9" s="4">
@@ -1260,7 +1259,7 @@
       <c r="Q10" s="4">
         <v>21070</v>
       </c>
-      <c r="R10" s="11">
+      <c r="R10" s="4">
         <v>85834</v>
       </c>
       <c r="S10" s="4">
@@ -1325,7 +1324,7 @@
       <c r="Q11" s="4">
         <v>21914</v>
       </c>
-      <c r="R11" s="11">
+      <c r="R11" s="4">
         <v>135996</v>
       </c>
       <c r="S11" s="4">
@@ -1390,7 +1389,7 @@
       <c r="Q12" s="4">
         <v>21304</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="4">
         <v>80982</v>
       </c>
       <c r="S12" s="4">
@@ -1455,7 +1454,7 @@
       <c r="Q13" s="4">
         <v>20925</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="4">
         <v>94907</v>
       </c>
       <c r="S13" s="4">
@@ -1520,7 +1519,7 @@
       <c r="Q14" s="4">
         <v>22345</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="4">
         <v>121499</v>
       </c>
       <c r="S14" s="4">
@@ -1585,7 +1584,7 @@
       <c r="Q15" s="4">
         <v>22754</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="4">
         <v>128692</v>
       </c>
       <c r="S15" s="4">
@@ -1650,7 +1649,7 @@
       <c r="Q16" s="4">
         <v>21025</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="4">
         <v>101590</v>
       </c>
       <c r="S16" s="4">
@@ -1715,7 +1714,7 @@
       <c r="Q17" s="4">
         <v>22570</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="4">
         <v>75024</v>
       </c>
       <c r="S17" s="4">
@@ -1780,7 +1779,7 @@
       <c r="Q18" s="4">
         <v>21563</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="4">
         <v>38647</v>
       </c>
       <c r="S18" s="4">

</xml_diff>

<commit_message>
edited Labor Productivity 2012/2015
dinivide sa 100 yung values
</commit_message>
<xml_diff>
--- a/Documentation/DataV3.xlsx
+++ b/Documentation/DataV3.xlsx
@@ -273,9 +273,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,8 +601,8 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S6" sqref="S6"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +686,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -702,7 +706,7 @@
       <c r="F2" s="7">
         <v>3019</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>236.06</v>
       </c>
       <c r="H2" s="3">
@@ -740,14 +744,16 @@
         <v>25007</v>
       </c>
       <c r="R2" s="4">
-        <v>501123</v>
+        <f>501123/100</f>
+        <v>5011.2299999999996</v>
       </c>
       <c r="S2" s="4">
-        <v>583368</v>
+        <f>583368/100</f>
+        <v>5833.68</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -767,7 +773,7 @@
       <c r="F3" s="7">
         <v>1170</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="10">
         <v>5024.1899999999996</v>
       </c>
       <c r="H3" s="3">
@@ -805,14 +811,16 @@
         <v>20448</v>
       </c>
       <c r="R3" s="4">
-        <v>103184</v>
+        <f>103184/100</f>
+        <v>1031.8399999999999</v>
       </c>
       <c r="S3" s="4">
-        <v>117327</v>
+        <f>117327/100</f>
+        <v>1173.27</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -832,7 +840,7 @@
       <c r="F4" s="7">
         <v>402</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="10">
         <v>7498.89</v>
       </c>
       <c r="H4" s="3">
@@ -870,14 +878,16 @@
         <v>21770</v>
       </c>
       <c r="R4" s="4">
-        <v>162642</v>
+        <f>162642/100</f>
+        <v>1626.42</v>
       </c>
       <c r="S4" s="4">
-        <v>175870</v>
+        <f>175870/100</f>
+        <v>1758.7</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -897,7 +907,7 @@
       <c r="F5" s="7">
         <v>816</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="10">
         <v>10899.21</v>
       </c>
       <c r="H5" s="3">
@@ -935,14 +945,16 @@
         <v>21860</v>
       </c>
       <c r="R5" s="4">
-        <v>78027</v>
+        <f>78027/100</f>
+        <v>780.27</v>
       </c>
       <c r="S5" s="4">
-        <v>88532</v>
+        <f>88532/100</f>
+        <v>885.32</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -962,7 +974,7 @@
       <c r="F6" s="7">
         <v>2507</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="10">
         <v>8499.9</v>
       </c>
       <c r="H6" s="3">
@@ -1000,14 +1012,16 @@
         <v>23200</v>
       </c>
       <c r="R6" s="4">
-        <v>151196</v>
+        <f>151196/100</f>
+        <v>1511.96</v>
       </c>
       <c r="S6" s="4">
-        <v>170684</v>
+        <f>170684/100</f>
+        <v>1706.84</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1027,7 +1041,7 @@
       <c r="F7" s="7">
         <v>3251</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="10">
         <v>6514.82</v>
       </c>
       <c r="H7" s="3">
@@ -1065,14 +1079,16 @@
         <v>22121</v>
       </c>
       <c r="R7" s="4">
-        <v>230968</v>
+        <f>230968/100</f>
+        <v>2309.6799999999998</v>
       </c>
       <c r="S7" s="4">
-        <v>256386</v>
+        <f>256386/100</f>
+        <v>2563.86</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1092,7 +1108,7 @@
       <c r="F8" s="7">
         <v>697</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="10">
         <v>11436.69</v>
       </c>
       <c r="H8" s="3">
@@ -1130,14 +1146,16 @@
         <v>20224</v>
       </c>
       <c r="R8" s="4">
-        <v>8618</v>
+        <f>8618/100</f>
+        <v>86.18</v>
       </c>
       <c r="S8" s="4">
-        <v>94144</v>
+        <f>94144/100</f>
+        <v>941.44</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1157,7 +1175,7 @@
       <c r="F9" s="7">
         <v>1262</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="10">
         <v>7010</v>
       </c>
       <c r="H9" s="3">
@@ -1195,14 +1213,16 @@
         <v>21476</v>
       </c>
       <c r="R9" s="4">
-        <v>55798</v>
+        <f>55798/100</f>
+        <v>557.98</v>
       </c>
       <c r="S9" s="4">
-        <v>65196</v>
+        <f>65196/100</f>
+        <v>651.96</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1222,7 +1242,7 @@
       <c r="F10" s="7">
         <v>1699</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="10">
         <v>4953.29</v>
       </c>
       <c r="H10" s="3">
@@ -1260,14 +1280,16 @@
         <v>21070</v>
       </c>
       <c r="R10" s="4">
-        <v>85834</v>
+        <f>85834/100</f>
+        <v>858.34</v>
       </c>
       <c r="S10" s="4">
-        <v>95211</v>
+        <f>95211/100</f>
+        <v>952.11</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1287,7 +1309,7 @@
       <c r="F11" s="7">
         <v>1672</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="10">
         <v>3900.47</v>
       </c>
       <c r="H11" s="3">
@@ -1325,14 +1347,16 @@
         <v>21914</v>
       </c>
       <c r="R11" s="4">
-        <v>135996</v>
+        <f>135996/100</f>
+        <v>1359.96</v>
       </c>
       <c r="S11" s="4">
-        <v>150228</v>
+        <f>150228/100</f>
+        <v>1502.28</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1352,7 +1376,7 @@
       <c r="F12" s="7">
         <v>976</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="10">
         <v>8977.2999999999993</v>
       </c>
       <c r="H12" s="3">
@@ -1390,14 +1414,16 @@
         <v>21304</v>
       </c>
       <c r="R12" s="4">
-        <v>80982</v>
+        <f>80982/100</f>
+        <v>809.82</v>
       </c>
       <c r="S12" s="4">
-        <v>150555</v>
+        <f>150555/100</f>
+        <v>1505.55</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1417,7 +1443,7 @@
       <c r="F13" s="7">
         <v>824</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="10">
         <v>6585.64</v>
       </c>
       <c r="H13" s="3">
@@ -1455,14 +1481,16 @@
         <v>20925</v>
       </c>
       <c r="R13" s="4">
-        <v>94907</v>
+        <f>94907/100</f>
+        <v>949.07</v>
       </c>
       <c r="S13" s="4">
-        <v>113384</v>
+        <f>113384/100</f>
+        <v>1133.8399999999999</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1482,7 +1510,7 @@
       <c r="F14" s="7">
         <v>1029</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="10">
         <v>7913.56</v>
       </c>
       <c r="H14" s="3">
@@ -1520,14 +1548,16 @@
         <v>22345</v>
       </c>
       <c r="R14" s="4">
-        <v>121499</v>
+        <f>121499/100</f>
+        <v>1214.99</v>
       </c>
       <c r="S14" s="4">
-        <v>142402</v>
+        <f>142402/100</f>
+        <v>1424.02</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1547,7 +1577,7 @@
       <c r="F15" s="7">
         <v>1156</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="10">
         <v>7860.04</v>
       </c>
       <c r="H15" s="3">
@@ -1585,14 +1615,16 @@
         <v>22754</v>
       </c>
       <c r="R15" s="4">
-        <v>128692</v>
+        <f>128692/100</f>
+        <v>1286.92</v>
       </c>
       <c r="S15" s="4">
-        <v>157780</v>
+        <f>157780/100</f>
+        <v>1577.8</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1612,7 +1644,7 @@
       <c r="F16" s="7">
         <v>1055</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="10">
         <v>8692.43</v>
       </c>
       <c r="H16" s="3">
@@ -1650,14 +1682,16 @@
         <v>21025</v>
       </c>
       <c r="R16" s="4">
-        <v>101590</v>
+        <f>101590/100</f>
+        <v>1015.9</v>
       </c>
       <c r="S16" s="4">
-        <v>115772</v>
+        <f>115772/100</f>
+        <v>1157.72</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1677,7 +1711,7 @@
       <c r="F17" s="7">
         <v>579</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="10">
         <v>8292.84</v>
       </c>
       <c r="H17" s="3">
@@ -1715,14 +1749,16 @@
         <v>22570</v>
       </c>
       <c r="R17" s="4">
-        <v>75024</v>
+        <f>75024/100</f>
+        <v>750.24</v>
       </c>
       <c r="S17" s="4">
-        <v>88178</v>
+        <f>88178/100</f>
+        <v>881.78</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1742,7 +1778,7 @@
       <c r="F18" s="7">
         <v>616</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="10">
         <v>4840.1000000000004</v>
       </c>
       <c r="H18" s="3">
@@ -1780,10 +1816,12 @@
         <v>21563</v>
       </c>
       <c r="R18" s="4">
-        <v>38647</v>
+        <f>38647/100</f>
+        <v>386.47</v>
       </c>
       <c r="S18" s="4">
-        <v>40008</v>
+        <f>40008/100</f>
+        <v>400.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data for number of out-of-school the ages 6 -24
</commit_message>
<xml_diff>
--- a/Documentation/DataV3.xlsx
+++ b/Documentation/DataV3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Desktop\IBMDESC-Poverty\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\IBMDESC-Poverty\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Region</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>LaborProductivity2015</t>
+  </si>
+  <si>
+    <t>NumberOfOutOfSchool6to24</t>
+  </si>
+  <si>
+    <t>NoOfSchool</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,6 +288,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -598,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,9 +631,11 @@
     <col min="17" max="17" width="26.42578125" customWidth="1"/>
     <col min="18" max="18" width="27.5703125" customWidth="1"/>
     <col min="19" max="19" width="29.5703125" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -684,8 +693,14 @@
       <c r="S1" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -751,8 +766,11 @@
         <f>583368/100</f>
         <v>5833.68</v>
       </c>
+      <c r="T2" s="11">
+        <v>4556</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -818,8 +836,11 @@
         <f>117327/100</f>
         <v>1173.27</v>
       </c>
+      <c r="T3" s="11">
+        <v>1806</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -885,8 +906,11 @@
         <f>175870/100</f>
         <v>1758.7</v>
       </c>
+      <c r="T4" s="11">
+        <v>681</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -952,8 +976,11 @@
         <f>88532/100</f>
         <v>885.32</v>
       </c>
+      <c r="T5" s="11">
+        <v>1261</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1019,8 +1046,11 @@
         <f>170684/100</f>
         <v>1706.84</v>
       </c>
+      <c r="T6" s="11">
+        <v>4060</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1086,8 +1116,11 @@
         <f>256386/100</f>
         <v>2563.86</v>
       </c>
+      <c r="T7" s="11">
+        <v>5209</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>49</v>
       </c>
@@ -1153,8 +1186,11 @@
         <f>94144/100</f>
         <v>941.44</v>
       </c>
+      <c r="T8" s="11">
+        <v>1189</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1220,8 +1256,11 @@
         <f>65196/100</f>
         <v>651.96</v>
       </c>
+      <c r="T9" s="11">
+        <v>2344</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1287,8 +1326,11 @@
         <f>95211/100</f>
         <v>952.11</v>
       </c>
+      <c r="T10" s="11">
+        <v>2832</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1354,8 +1396,11 @@
         <f>150228/100</f>
         <v>1502.28</v>
       </c>
+      <c r="T11" s="11">
+        <v>2776</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1421,8 +1466,9 @@
         <f>150555/100</f>
         <v>1505.55</v>
       </c>
+      <c r="T12" s="11"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
@@ -1488,8 +1534,11 @@
         <f>113384/100</f>
         <v>1133.8399999999999</v>
       </c>
+      <c r="T13" s="11">
+        <v>1475</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1555,8 +1604,11 @@
         <f>142402/100</f>
         <v>1424.02</v>
       </c>
+      <c r="T14" s="11">
+        <v>1846</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
@@ -1622,8 +1674,11 @@
         <f>157780/100</f>
         <v>1577.8</v>
       </c>
+      <c r="T15" s="11">
+        <v>1862</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1689,8 +1744,11 @@
         <f>115772/100</f>
         <v>1157.72</v>
       </c>
+      <c r="T16" s="11">
+        <v>1791</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
@@ -1756,8 +1814,11 @@
         <f>88178/100</f>
         <v>881.78</v>
       </c>
+      <c r="T17" s="11">
+        <v>1039</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>31</v>
       </c>
@@ -1822,6 +1883,9 @@
       <c r="S18" s="4">
         <f>40008/100</f>
         <v>400.08</v>
+      </c>
+      <c r="T18" s="11">
+        <v>1511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added analysis and add number of school data
</commit_message>
<xml_diff>
--- a/Documentation/DataV3.xlsx
+++ b/Documentation/DataV3.xlsx
@@ -260,7 +260,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,7 +288,6 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -607,9 +606,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,8 +765,11 @@
         <f>583368/100</f>
         <v>5833.68</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="4">
         <v>4556</v>
+      </c>
+      <c r="U2" s="4">
+        <v>768</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -836,8 +838,11 @@
         <f>117327/100</f>
         <v>1173.27</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="4">
         <v>1806</v>
+      </c>
+      <c r="U3" s="4">
+        <v>2926</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -906,8 +911,11 @@
         <f>175870/100</f>
         <v>1758.7</v>
       </c>
-      <c r="T4" s="11">
+      <c r="T4" s="4">
         <v>681</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1816</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -976,8 +984,11 @@
         <f>88532/100</f>
         <v>885.32</v>
       </c>
-      <c r="T5" s="11">
+      <c r="T5" s="4">
         <v>1261</v>
+      </c>
+      <c r="U5" s="4">
+        <v>2583</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1046,8 +1057,11 @@
         <f>170684/100</f>
         <v>1706.84</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T6" s="4">
         <v>4060</v>
+      </c>
+      <c r="U6" s="4">
+        <v>3621</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1116,8 +1130,11 @@
         <f>256386/100</f>
         <v>2563.86</v>
       </c>
-      <c r="T7" s="11">
+      <c r="T7" s="4">
         <v>5209</v>
+      </c>
+      <c r="U7" s="4">
+        <v>3392</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1186,8 +1203,11 @@
         <f>94144/100</f>
         <v>941.44</v>
       </c>
-      <c r="T8" s="11">
+      <c r="T8" s="4">
         <v>1189</v>
+      </c>
+      <c r="U8" s="4">
+        <v>2198</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1256,8 +1276,11 @@
         <f>65196/100</f>
         <v>651.96</v>
       </c>
-      <c r="T9" s="11">
+      <c r="T9" s="4">
         <v>2344</v>
+      </c>
+      <c r="U9" s="4">
+        <v>3798</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1326,8 +1349,11 @@
         <f>95211/100</f>
         <v>952.11</v>
       </c>
-      <c r="T10" s="11">
+      <c r="T10" s="4">
         <v>2832</v>
+      </c>
+      <c r="U10" s="4">
+        <v>4050</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1396,8 +1422,11 @@
         <f>150228/100</f>
         <v>1502.28</v>
       </c>
-      <c r="T11" s="11">
+      <c r="T11" s="4">
         <v>2776</v>
+      </c>
+      <c r="U11" s="4">
+        <v>3737</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1466,7 +1495,10 @@
         <f>150555/100</f>
         <v>1505.55</v>
       </c>
-      <c r="T12" s="11"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4">
+        <v>4132</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1534,8 +1566,11 @@
         <f>113384/100</f>
         <v>1133.8399999999999</v>
       </c>
-      <c r="T13" s="11">
+      <c r="T13" s="4">
         <v>1475</v>
+      </c>
+      <c r="U13" s="4">
+        <v>2488</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1604,8 +1639,11 @@
         <f>142402/100</f>
         <v>1424.02</v>
       </c>
-      <c r="T14" s="11">
+      <c r="T14" s="4">
         <v>1846</v>
+      </c>
+      <c r="U14" s="4">
+        <v>2441</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1674,8 +1712,11 @@
         <f>157780/100</f>
         <v>1577.8</v>
       </c>
-      <c r="T15" s="11">
+      <c r="T15" s="4">
         <v>1862</v>
+      </c>
+      <c r="U15" s="4">
+        <v>1933</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1744,11 +1785,14 @@
         <f>115772/100</f>
         <v>1157.72</v>
       </c>
-      <c r="T16" s="11">
+      <c r="T16" s="4">
         <v>1791</v>
       </c>
+      <c r="U16" s="4">
+        <v>2168</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
@@ -1814,11 +1858,14 @@
         <f>88178/100</f>
         <v>881.78</v>
       </c>
-      <c r="T17" s="11">
+      <c r="T17" s="4">
         <v>1039</v>
       </c>
+      <c r="U17" s="4">
+        <v>2038</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>31</v>
       </c>
@@ -1884,8 +1931,11 @@
         <f>40008/100</f>
         <v>400.08</v>
       </c>
-      <c r="T18" s="11">
+      <c r="T18" s="4">
         <v>1511</v>
+      </c>
+      <c r="U18" s="4">
+        <v>2514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>